<commit_message>
srds and presentation stuff
</commit_message>
<xml_diff>
--- a/JCSC_SOURCE_MATRIX.xlsx
+++ b/JCSC_SOURCE_MATRIX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\JCSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9BC684-3F5E-42CD-BE1C-5D672C6BD847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D06BD92-D741-4397-BDA1-75D0FE1258C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9A08C367-70A1-4CB7-9B0B-0DF2B9CEDD0C}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9A08C367-70A1-4CB7-9B0B-0DF2B9CEDD0C}"/>
   </bookViews>
   <sheets>
     <sheet name="MATRIX DATA" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4308" uniqueCount="4231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4594" uniqueCount="4515">
   <si>
     <t>Author</t>
   </si>
@@ -13483,6 +13483,858 @@
   </si>
   <si>
     <t>EDSTROM_2023</t>
+  </si>
+  <si>
+    <t>Richard K. Betts</t>
+  </si>
+  <si>
+    <t>Collective security’s logic and limits; arms control’s fit after the Cold War</t>
+  </si>
+  <si>
+    <t>Conceptual analysis with systems-theory framing; historical counter-examples; realist benchmarks (L11–L17, L43–L56)</t>
+  </si>
+  <si>
+    <t>Core claim: enthusiasm confuses cause and effect; collective security either fails when needed or, if honoured, can widen wars (L43–L69)</t>
+  </si>
+  <si>
+    <t>Key ideas: automaticity and universality define true collective security; legalism vs balance; flexibility–power trade-off; alliance “shells”; Concert de-collectivises; areas of “special interest” (L44–L51; L31–L43; L31–L40; L31–L43; L30–L36)</t>
+  </si>
+  <si>
+    <t>Strengths: sharp definitions; clear trade-offs; telling historical vignettes; testable cautions (L44–L51; L31–L40; L55–L67)</t>
+  </si>
+  <si>
+    <t>Weaknesses: realist tilt; thin empirical testing; analogy reliance; dated post–Cold War assumptions (general)</t>
+  </si>
+  <si>
+    <t>Similarities: converges with structural realist scepticism about legalist schemes (L3–L19)</t>
+  </si>
+  <si>
+    <t>Differences: diverges from liberal “limited collective security” proposals and post-national optimism (L69–L73; L12–L20)</t>
+  </si>
+  <si>
+    <t>Notes: “peace will cause peace rather than collective security will cause peace”; “if it works, we may wish it hadn’t” (L57–L63; L59–L69)</t>
+  </si>
+  <si>
+    <t>My conclusion: use Betts to interrogate advocacy texts; demand automaticity or call it balancing; test causal claims</t>
+  </si>
+  <si>
+    <t>Realist academic at Columbia; incentive to puncture idealist orthodoxy; audience is policy and scholarly (L68–L75)</t>
+  </si>
+  <si>
+    <t>Key limitations: no micro-data; Europe since 1992 changed; efficacy claims remain conditional (general)</t>
+  </si>
+  <si>
+    <t>D_Describe: Reframes collective security as an emergency system whose design rarely fits crises; warns of perverse effects (L11–L17; L59–L69).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Matters for thesis because it exposes rhetorical drift from law-like ideals to interest-based practice (L44–L51).</t>
+  </si>
+  <si>
+    <t>D_Methodology: Conceptual critique with systems analogies and historical contrasts; moderate external validity (L11–L17; L59–L67).</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Bite: automaticity–universality as falsifier of “collective” claims (L44–L51); Falsifier: show durable automatic, universal compliance without great-power tutelage.</t>
+  </si>
+  <si>
+    <t>D_Author: Realist lens; sceptical of legalism; Really saying: peace follows interests, not slogans (L19–L27; L31–L33).</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with Morgenthau/Kennan cautions; diverges from Ullman/Kupchan buffers and “areas of interest” (L30–L36; L15–L26).</t>
+  </si>
+  <si>
+    <t>D_Limit: Pre-1992 context; under-reads institutional learning.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF: prioritise flexible coalitions, legal-evidence skills and resilience over slogans.</t>
+  </si>
+  <si>
+    <t>BETTS_1992</t>
+  </si>
+  <si>
+    <t>Jean-Loup Samaan</t>
+  </si>
+  <si>
+    <t>Small-state strategic autonomy; UAE–Singapore comparison; self-reliance vs patronage</t>
+  </si>
+  <si>
+    <t>Comparative analysis of policy, force, and industry; balances “false uniqueness” and “false universalism” (pp.110–111)</t>
+  </si>
+  <si>
+    <t>Autonomy is a constant bargain; both depend on the US; industry can do niches not major platforms; policies diverge yet are fragile under US–China stress (pp.118–119)</t>
+  </si>
+  <si>
+    <t>Key ideas: autonomy defined as independent planning, operations, and capabilities; vulnerability–agency paradox; EDGE and ST Engineering as compromise models; national service trajectories differ (pp.110–114, 116–118)</t>
+  </si>
+  <si>
+    <t>Strengths: clear definition and scope; cross-regional comparison; granular industry examples; explicit boundary conditions (pp.110–114, 118)</t>
+  </si>
+  <si>
+    <t>Weaknesses: reliance on public sources; limited causal testing; uncertain UAE conscription effects (p.116)</t>
+  </si>
+  <si>
+    <t>Similarities: shared constraints; US as external balancer; niche industrial focus (pp.118–119)</t>
+  </si>
+  <si>
+    <t>Differences: Singapore embeds self-reliance early and stays cautious; UAE diversifies and tests limits (pp.118–119)</t>
+  </si>
+  <si>
+    <t>Notes: EDGE absorbs EDIC in 2019; AMMROC JV upgrades; ST Engineering scale and focus; Singapore upgrades over new buys (pp.113–114)</t>
+  </si>
+  <si>
+    <t>My conclusion: use as a small-state typology; test Irish exposure, human capital, industry, patron options before inferring autonomy</t>
+  </si>
+  <si>
+    <t>Academic at NUS; prior roles with NATO and UAE NDC; policy-analytic lens; likely incentive to discipline autonomy rhetoric (p.123)</t>
+  </si>
+  <si>
+    <t>Key Limitations: declaratory sources; industrial self-sufficiency bounded; UAE NS outcome data thin (pp.114, 116)</t>
+  </si>
+  <si>
+    <t>D_Describe: Compares UAE and Singapore; autonomy is a moving bargain, not a status (p.119).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Shows exposure and patron choices shape autonomy; Europe-centric debates under-specify this (pp.110–112).</t>
+  </si>
+  <si>
+    <t>D_Methodology: Documented comparison with industry cases; balances uniqueness vs universalism; moderate validity (pp.110–111).</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Bite: autonomy ceiling in industry and alliances; falsifier: sustained major-platform indigenisation without patrons (pp.114, 118–119).</t>
+  </si>
+  <si>
+    <t>D_Author: NUS scholar with Gulf focus; Really saying: tailor self-reliance to size, exposure, patron leeway (p.123).</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Converges with realist exposure logic; diverges from post-national optimism on European autonomy (pp.110–112).</t>
+  </si>
+  <si>
+    <t>D_Limit: Public-source bias; unclear UAE NS impact; causality tentative (p.116).</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF balances expeditionary interoperability with resilience and evidence-ready logistics for shocks.</t>
+  </si>
+  <si>
+    <t>Rebecca L. Schiff</t>
+  </si>
+  <si>
+    <t>Civil–military relations; concordance theory vs separation</t>
+  </si>
+  <si>
+    <t>Conceptual theory with brief comparative cases (Israel, India); descriptive–prescriptive</t>
+  </si>
+  <si>
+    <t>Agreement among military, political elites and citizenry on four indicators lowers likelihood of domestic military intervention (pp.9–13)</t>
+  </si>
+  <si>
+    <t>Four indicators: officer corps composition; political decision-making; recruitment method; military style; culture central; multiple patterns incl. integration (p.13; pp.16–17)</t>
+  </si>
+  <si>
+    <t>Integrates culture with institutions; predictive frame; challenges US-centric assumptions; two clear cases</t>
+  </si>
+  <si>
+    <t>Light empirical testing; selection bias; limited operationalisation; dated cases</t>
+  </si>
+  <si>
+    <t>Converges with culturalist and sociological takes on civil–military relations</t>
+  </si>
+  <si>
+    <t>Differs from strict separation models; adds citizenry and style as core variables</t>
+  </si>
+  <si>
+    <t>Israel shows “uncivil” mix yet no coups; India’s weakening civil centre still no intervention; style and recruitment matter (pp.19–21)</t>
+  </si>
+  <si>
+    <t>Use concordance as a diagnostic for small states; map Ireland’s four indicators before reform</t>
+  </si>
+  <si>
+    <t>Author critiques dominant US model; early-career incentive to propose alternative; policy–academic audience</t>
+  </si>
+  <si>
+    <t>Two positive cases only; lacks disconfirming cases; measurement thin</t>
+  </si>
+  <si>
+    <t>D_Describe: Concordance on four indicators reduces intervention (pp.9–13).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Recasts control as cultural agreement; omits measurement detail.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Conceptual synthesis plus case sketches; moderate validity.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest bite is testable four-indicator claim (p.13); Falsifier: agreement yet coup occurs.</t>
+  </si>
+  <si>
+    <t>D_Author: Critical of separation; policy audience; Really saying: context first, form varies.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with culturalists; diverges from Huntington on strict separation.</t>
+  </si>
+  <si>
+    <t>D_Limit: Thin operationalisation and dated evidence.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF should build cross-societal concordance on recruitment, style and decision paths.</t>
+  </si>
+  <si>
+    <t>SCHIFF_1995</t>
+  </si>
+  <si>
+    <t>SAMAAN_2025</t>
+  </si>
+  <si>
+    <t>Concordance theory and targeted partnership in civil–military relations</t>
+  </si>
+  <si>
+    <t>Commentary; retrospective synthesis with policy reflections</t>
+  </si>
+  <si>
+    <t>Concordance frames prevention of domestic military intervention via agreement among partners on four indicators; targeted partnership offers short-term civil–military collaboration (pp. 520–521)</t>
+  </si>
+  <si>
+    <t>Three partners and four indicators; Israeli case; NATO RTG-HFM-226 link; Petraeus JSAT and PRTs as examples; critique of Huntington’s separation model (pp. 520–522)</t>
+  </si>
+  <si>
+    <t>Conceptual clarity; policy traction via NATO and PRT examples; culturally sensitive framing (pp. 520–522)</t>
+  </si>
+  <si>
+    <t>Limited new evidence; polemical tone on academy politics; no systematic counter-testing; case selection risk (pp. 519–522)</t>
+  </si>
+  <si>
+    <t>Aligns with institutional-cultural CMR approaches</t>
+  </si>
+  <si>
+    <t>Diverts from Huntington’s objective control separation doctrine</t>
+  </si>
+  <si>
+    <t>Useful lens for small-state state-building tasks and DF civil–military liaison; treat anti-coup claims cautiously (pp. 520–522)</t>
+  </si>
+  <si>
+    <t>Adopt concordance as a diagnostic and targeted partnership as a pragmatic tool in UN-EU missions; measure agreement against indicators (pp. 520–521)</t>
+  </si>
+  <si>
+    <t>Advocates Israel as validating case; critiques US academic reception; policy-engaged stance (pp. 519–522)</t>
+  </si>
+  <si>
+    <t>Commentary genre; absence of measurable tests; generalisability unproven (pp. 520–522)</t>
+  </si>
+  <si>
+    <t>D_Describe: Concordance prevents domestic intervention if partners agree on four indicators (p. 520).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Relevance lies in culturally grounded anti-coup prediction; omits systematic falsification.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Retrospective commentary drawing on prior cases and NATO practice; moderate validity.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest on four indicators synthesis (p. 520); Falsifier: if coups occur under full indicator concordance.</t>
+  </si>
+  <si>
+    <t>D_Author: Pro-concordance, pro-Israel, policy-practitioner lens; Really saying: culture plus institutions avert coups.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Converges with institutionalists; diverges from Huntington’s strict separation due to Israeli case.</t>
+  </si>
+  <si>
+    <t>D_Limit: No fresh data or cross-case metrics.</t>
+  </si>
+  <si>
+    <t>D_Implication: DF should map partner agreement and build targeted partnerships in peace support.</t>
+  </si>
+  <si>
+    <t>SCHIFF_2025</t>
+  </si>
+  <si>
+    <t>Concordance theory rebuttal to Wells; four indicators and three partners prevent domestic military intervention</t>
+  </si>
+  <si>
+    <t>Conceptual rejoinder using deductive causation; illustrative cases Israel and India (pp. 277–282)</t>
+  </si>
+  <si>
+    <t>Agreement among political elites, military, and citizenry on social composition, decision-making, recruitment, and military style lowers coup risk (pp. 277–278)</t>
+  </si>
+  <si>
+    <t>Four indicators; three partners; culture counts; US can mix institutions without coups; concordance predicts conditions not one model (pp. 277–281)</t>
+  </si>
+  <si>
+    <t>Sharp causal claim; engages critics directly; culturally sensitive; applies to varied cases including US, Israel, India (pp. 277–282)</t>
+  </si>
+  <si>
+    <t>Thin empirical testing; operationalisation light; risks post-hoc reading; business analogies stretch scope (pp. 282–283)</t>
+  </si>
+  <si>
+    <t>Converges with Kohn on low US coup risk and with cultural approaches in civil–military studies (p. 280)</t>
+  </si>
+  <si>
+    <t>Differs from Huntington’s separation thesis; rejects presumption that militaries are innately coercive (pp. 278–281)</t>
+  </si>
+  <si>
+    <t>US overlap without intervention weakens separation theory; Israel’s fusion without coups; India’s professionalism despite weak civilians (pp. 279–282)</t>
+  </si>
+  <si>
+    <t>Use concordance as a flexible lens for small states; test indicators against Irish context before structural change (pp. 277–282)</t>
+  </si>
+  <si>
+    <t>Originator defending her theory; entrepreneurial application to business suggests advocacy stance (p. 277, p. 283)</t>
+  </si>
+  <si>
+    <t>Limited falsifiers stated; few cases; measurement of “agreement” unclear (pp. 277–283)</t>
+  </si>
+  <si>
+    <t>D_Describe: Reasserts four-indicator concordance prevents domestic intervention, countering Wells (pp. 277–278).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Matters as a culturally aware brake on importing US separation models; omits robust metrics.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Theoretical rejoinder with deductive causation and cases; validity moderate; bias likely.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest bite is US overlap without coups (p. 280); Falsifier: if sustained overlap correlates with coup attempts.</t>
+  </si>
+  <si>
+    <t>D_Author: Pro-concordance, academic-policy lens, advocacy to business; really saying: culture plus institutional agreement beats tidy separation.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with culturalists and Kohn on low coup risk; diverges from Huntington’s objective control.</t>
+  </si>
+  <si>
+    <t>D_Limit: Few cases and no clear thresholds to code concordance.</t>
+  </si>
+  <si>
+    <t>D_Implication: For DF, seek visible elite–military–society alignment on role, recruitment, and style before major reforms.</t>
+  </si>
+  <si>
+    <t>SCHIFF_1996</t>
+  </si>
+  <si>
+    <t>David Kuehn; Philip Lorenz</t>
+  </si>
+  <si>
+    <t>Explaining civil–military relations in new democracies; structure–agency and theory development</t>
+  </si>
+  <si>
+    <t>Meta-theoretical analysis; conceptual mapping; comparative critique of four integrative theories</t>
+  </si>
+  <si>
+    <t>Systematises actors–environment–linkage; finds no approach fully integrates structure and agency; urges explicit mechanisms for testable hypotheses (pp.243–245)</t>
+  </si>
+  <si>
+    <t>Structure–agency problem; entities–environment–relationship triad; feasible set and decision rule; constraints vs generative vs resource models; structured contingency; complexity trade-off</t>
+  </si>
+  <si>
+    <t>Theory map is clear; integrates literatures; offers criteria for completeness; practical checklist for hypothesis design</t>
+  </si>
+  <si>
+    <t>Abstract, no new data; four-theory selection; limited operationalisation; variable lists remain broad</t>
+  </si>
+  <si>
+    <t>Aligns with integrative CMR work seeking mechanisms and strategies</t>
+  </si>
+  <si>
+    <t>Differs from single-factor or separation-only models; treats structure and agency as co-constitutive</t>
+  </si>
+  <si>
+    <t>Use as slide-ready template: specify agents, environments, mechanism, strategy set, decision rule before claims</t>
+  </si>
+  <si>
+    <t>My conclusion: adopt structured contingency lens; design DSS claims with explicit mechanism and condition</t>
+  </si>
+  <si>
+    <t>Heidelberg PhD researchers; theory-building incentive; philosophy-of-science lens; academic audience. Really saying: specify actors and mechanisms or claims wobble</t>
+  </si>
+  <si>
+    <t>Lacks empirical testing; no full variable inventory; relies on selected cases; measures thin</t>
+  </si>
+  <si>
+    <t>D_Describe: Maps structure–agency and tests four theories’ completeness (pp.231–233).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Completeness matters for clear hypotheses; omission blurs predictions.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Meta-theory plus comparative critique; moderate validity; no new data.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Best bite is three-step template (p.245); Falsifier: a theory meets all steps yet fails.</t>
+  </si>
+  <si>
+    <t>D_Author: Theory-first stance; building-blocks incentive; Really saying: mechanisms before metrics.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Places Alagappa near structure and Trinkunas near agency with gaps.</t>
+  </si>
+  <si>
+    <t>D_Limit: Theorised, not tested.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF claims must state agents, environments, causal link before policy.</t>
+  </si>
+  <si>
+    <t>KUEHN_2011</t>
+  </si>
+  <si>
+    <t>Valery Gerasimov</t>
+  </si>
+  <si>
+    <t>The Value of Science Is in the Foresight; Russian general staff view of modern conflict</t>
+  </si>
+  <si>
+    <t>Conceptual essay; strategic reflection using recent conflicts and colour revolutions</t>
+  </si>
+  <si>
+    <t>War has blurred with politics; non-military means can outweigh force; integrated whole-of-government needed (pp.23–25)</t>
+  </si>
+  <si>
+    <t>Non-military means sometimes exceed weapons; information struggle central; preemption and constant pressure; unified command; rapid adaptation (pp.23–27)</t>
+  </si>
+  <si>
+    <t>Insider view; concise articulation of Russian military-scientific discourse; early synthesis of information-centric conflict</t>
+  </si>
+  <si>
+    <t>Normative, not empirical; ambiguous terms; translation artefacts; misread as doctrine; little falsifiable evidence</t>
+  </si>
+  <si>
+    <t>Converges with Chekinov–Bogdanov on information dominance and strategic shaping</t>
+  </si>
+  <si>
+    <t>Diverts from Western hybrid-warfare frames by centring state-led, preemptive political warfare</t>
+  </si>
+  <si>
+    <t>Use as window into Russian strategic thought, not as binding doctrine; quote selectively with context (pp.23–29)</t>
+  </si>
+  <si>
+    <t>Treat as agenda-setting signal of priorities and anxieties, not a plan of operations</t>
+  </si>
+  <si>
+    <t>Serving CGS; institutional defence lens; incentive to justify resources and counter Western influence</t>
+  </si>
+  <si>
+    <t>No data tests; scope limited to selective cases; relies on assertions and exemplars</t>
+  </si>
+  <si>
+    <t>D_Describe: Argues non-military means can surpass force in modern conflict (pp.23–24).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Matters for Russian intent signalling; omits rigorous causal tests.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Programmatic essay using exemplars; validity limited, bias high.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest on information centrality (p.24); falsifier: if kinetic effects dominate across cases.</t>
+  </si>
+  <si>
+    <t>D_Author: State-security stance; CGS lens; incentive to expand remit. Really saying: integrate politics and war.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with Russian military science on information primacy; diverges from Western doctrinal takes.</t>
+  </si>
+  <si>
+    <t>D_Limit: Assertions lack comparative measurement.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF must harden info resilience and interagency coordination.</t>
+  </si>
+  <si>
+    <t>GERASIMOV_2016</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>The Future of Hybrid Warfare</t>
+  </si>
+  <si>
+    <t>Policy-analytical essay; conceptual synthesis across recent conflicts and statecraft tools (pp.1–5)</t>
+  </si>
+  <si>
+    <t>Hybrid warfare likely to persist as blending of conventional force, cyber, lawfare, disinfo and coercive economics (pp.1–3)</t>
+  </si>
+  <si>
+    <t>Hybrid toolset, threshold management, ambiguity as strategy, societal resilience as defence centre of gravity, role of alliances and legal frameworks (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Clear high-level map of instruments; policy relevance; concise horizon scan (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Thin empirical testing; few operational metrics; author and cases not specified; pages lack data tables (pp.1–5)</t>
+  </si>
+  <si>
+    <t>Aligns with NATO-EU emphasis on whole-of-society resilience and deterrence by denial (pp.3–4)</t>
+  </si>
+  <si>
+    <t>Differs from techno-determinist takes that privilege cyber alone; insists on multi-vector coercion (pp.2–3)</t>
+  </si>
+  <si>
+    <t>Notes on Irish context: maritime energy, data centres, diaspora influence, legal levers, neutrality signalling (pp.3–4)</t>
+  </si>
+  <si>
+    <t>My conclusion: treat hybrid pressure as chronic competition problem; prioritise resilience, attribution pathways, cross-government playbooks (pp.3–5)</t>
+  </si>
+  <si>
+    <t>Implicit Western security lens; policy-audience incentive; risk of confirmation bias toward state-led threat models (pp.1–5)</t>
+  </si>
+  <si>
+    <t>Key limitation: no comparative outcome data or thresholds for success/failure of tools (pp.2–5)</t>
+  </si>
+  <si>
+    <t>D_Describe: scans hybrid instruments and future trajectories; core claim is persistence and diffusion (pp.1–3).</t>
+  </si>
+  <si>
+    <t>D_Interpret: matters for thesis LO on critical synthesis and applied policy; omits measurement and Irish-specific baselines.</t>
+  </si>
+  <si>
+    <t>D_Methodology: narrative synthesis of cases and instruments; evidence impressionistic; validity moderate for scoping.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: strongest on instrument mapping and resilience levers (p.3); Falsifier: if cross-case metrics show pure kinetic dominance restores primacy.</t>
+  </si>
+  <si>
+    <t>D_Author: policy lens; likely aimed at officials; Really saying: build resilience and legal options, not gadgets.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: converges with resilience scholarship; diverges from narrow cyber-threat framings due to emphasis on society.</t>
+  </si>
+  <si>
+    <t>D_Limit: lacks method to score hybrid campaigns.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF invests in STRATCOM, attribution, legal pre-emption, inter-agency drills.</t>
+  </si>
+  <si>
+    <t>HOFFMAN_2024</t>
+  </si>
+  <si>
+    <t>Azad; Haider; Sadiq</t>
+  </si>
+  <si>
+    <t>Understanding Gray Zone Warfare from Multiple Perspectives</t>
+  </si>
+  <si>
+    <t>Conceptual synthesis of definitions plus brief comparative case illustrations (pp.5–6, 16–21)</t>
+  </si>
+  <si>
+    <t>Gray zone is a distinct domain below conventional war; tactics change status quo without crossing red lines; illustrated via Russia, China, Iran, India–Pakistan; concludes need for tailored counters (pp.5–6, 16–21)</t>
+  </si>
+  <si>
+    <t>Distinctness from hybrid warfare; below-threshold coercion; strategies include proxy war, fait accompli, salami tactics, information ops, cyber; cases: Crimea 2014, South China Sea, Iranian proxies, India–Pakistan escalation risks; countering concepts incl. modelling and AI (pp.6, 16–21)</t>
+  </si>
+  <si>
+    <t>Clarity on distinctness claim; spans state and NSA tactics; concise tour of diverse theatres; links tactics to status quo alteration (pp.5–6, 21)</t>
+  </si>
+  <si>
+    <t>Limited empirical testing; brief cases lack metrics; Western policy lens; sparse operational thresholds; little small-state doctrine detail (pp.16–21)</t>
+  </si>
+  <si>
+    <t>Aligns with literature that frames gray zone as below-threshold coercion; overlaps with hybrid concepts on tools used (pp.6, 21)</t>
+  </si>
+  <si>
+    <t>Differs from views that call gray zone a muddled rebrand; asserts conceptual distinctness and practical utility (p.5)</t>
+  </si>
+  <si>
+    <t>Use the distinctness claim to structure coding of cases; treat thresholds as contingent; do not universalise Russia/China patterns to small states (pp.5–6, 16–19)</t>
+  </si>
+  <si>
+    <t>Gray zone is best treated as a distinct analytic lens for below-threshold coercion; DF planning should emphasise attribution, resilience, calibrated responses (pp.6, 21)</t>
+  </si>
+  <si>
+    <t>Authors in UK institutions; policy–academic audience; incentive to clarify concept and inform Western practice; no funding stated. Really saying: treat gray zone as distinct and plan to counter below-threshold coercion (p.15)</t>
+  </si>
+  <si>
+    <t>Short on measurement and falsifiable criteria; cases primarily major-power led; limited Irish or EU small-state application detail (pp.16–21)</t>
+  </si>
+  <si>
+    <t>D_Describe: Gray zone is distinct; below-threshold coercion alters status quo (pp.5–6).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Clarifies concept for strategy; omits rigorous metrics.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Conceptual synthesis plus illustrative cases; moderate validity.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest bite is distinctness claim (p.5); Falsifier: if case coding cannot separate from hybrid warfare.</t>
+  </si>
+  <si>
+    <t>D_Author: UK policy–academic lens; clarify for practitioners. Really saying: plan for sub-threshold coercion.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Converges with Brands, Wirtz on coercive status-quo change.</t>
+  </si>
+  <si>
+    <t>D_Limit: Brief cases; few operational thresholds.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF needs attribution, resilience, calibrated escalation control.```</t>
+  </si>
+  <si>
+    <t>AZAD_2022</t>
+  </si>
+  <si>
+    <t>Libiseller</t>
+  </si>
+  <si>
+    <t>‘Hybrid warfare’ as an academic fashion</t>
+  </si>
+  <si>
+    <t>Conceptual critique with bibliometric cues; discourse analysis of strategic studies venues (n.p.)</t>
+  </si>
+  <si>
+    <t>Hybrid warfare functions as an academic fashion rather than a cumulative analytical concept; uptake is politicised and post-2014 surge reflects demand-pull from policy (n.p.)</t>
+  </si>
+  <si>
+    <t>Fashion cycles; concept stretching; policy–academia coupling; post-2014 popularity spike; limited operationalisation; caution for thesis framing (n.p.)</t>
+  </si>
+  <si>
+    <t>Coherent fashion lens; traces diffusion; links policy salience to academic uptake; sharp conceptual hygiene (n.p.)</t>
+  </si>
+  <si>
+    <t>Limited outcome measurement; probable English-language focus; selection risk; little predictive testing (n.p.)</t>
+  </si>
+  <si>
+    <t>Converges with sceptics who see continuity under new labels (n.p.)</t>
+  </si>
+  <si>
+    <t>Differs from novelty advocates who treat hybrid war as paradigmatic break (n.p.)</t>
+  </si>
+  <si>
+    <t>Use as a cautionary scaffold; define mechanisms precisely; avoid treating “hybrid” as an independent variable; ground claims in measurable effects (n.p.)</t>
+  </si>
+  <si>
+    <t>Treat hybrid warfare as a rhetorical umbrella; unpack concrete mechanisms and test them; privilege measurement over labels (n.p.)</t>
+  </si>
+  <si>
+    <t>Policy-sceptic academic stance; incentive to demystify buzzwords; audience is scholars and reflective practitioners (n.p.)</t>
+  </si>
+  <si>
+    <t>No cross-case metrics; narrow corpus; weak external validity (n.p.)</t>
+  </si>
+  <si>
+    <t>D_Describe: Shows hybrid warfare as academic fashion with politicised uptake after 2014 (n.p.).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Warns against fad-driven research; omits strong tests of explanatory power.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Conceptual critique plus bibliometric scan; moderate validity; context is policy salience.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest on fashion mechanism; falsifier: if precise hybrid measures predict outcomes better than rivals.</t>
+  </si>
+  <si>
+    <t>D_Author: Critical scholar; institutional lens wary of policy pull; Really saying: stop chasing buzzwords.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with continuity sceptics; diverges from transformation claims.</t>
+  </si>
+  <si>
+    <t>D_Limit: Lacks operational measures and cross-language coverage.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF should privilege concrete capability analysis and measurable effects over labels.</t>
+  </si>
+  <si>
+    <t>LIBISELLER_2023</t>
+  </si>
+  <si>
+    <t>REGAN_2024</t>
+  </si>
+  <si>
+    <t>Aurel Sari; Mitt Regan</t>
+  </si>
+  <si>
+    <t>Introduction to hybrid threats and grey zone conflict; conceptual clarification and scope (pp.10–12)</t>
+  </si>
+  <si>
+    <t>Conceptual synthesis; definitional framing using NATO and literature; policy triangulation</t>
+  </si>
+  <si>
+    <t>Hybrid threats and grey zone are complementary; grey zone is a band between war and peace; working definition offered (pp.10–11)</t>
+  </si>
+  <si>
+    <t>Below-threshold competition; ambiguity as tactic; complementarity not synonymy; zone not line; pejorative drift of 'hybrid threats'; strategic integration across domains (pp.10–12)</t>
+  </si>
+  <si>
+    <t>Clear synthesis; crisp working definition; bridges policy and scholarship; directly usable for strategy (pp.10–12)</t>
+  </si>
+  <si>
+    <t>Case-light; West-centric lens; potential vagueness if not operationalised; relies on policy rhetoric</t>
+  </si>
+  <si>
+    <t>Aligns with Mattis and Hoffman on blended modalities (p.12) and NATO on ambiguity (p.10)</t>
+  </si>
+  <si>
+    <t>Diverges from totalising 'hybrid war' and from critics who call terms empty; reframes threshold to zone and complementarity (p.11)</t>
+  </si>
+  <si>
+    <t>Notes NATO definition; 'hybrid threats' used as pejorative label for autocracies; volume aims to stabilise terms (pp.10–12)</t>
+  </si>
+  <si>
+    <t>Use definitions as scaffolding; set empirical indicators for grey zone band; map Irish vulnerabilities and instruments</t>
+  </si>
+  <si>
+    <t>Editors with Western academic policy lens; likely incentive to legitimise volume and orient debate; no funding stated</t>
+  </si>
+  <si>
+    <t>No measurement protocol for when tactics move from competitive to hostile; few cases; definitional reification risk</t>
+  </si>
+  <si>
+    <t>D_Describe: defines complementary concepts and a grey zone band between war and peace; proposes a working definition (p.11)</t>
+  </si>
+  <si>
+    <t>D_Interpret: clarifies planning and legal posture in below-threshold contests; omits measurement strategy</t>
+  </si>
+  <si>
+    <t>D_Methodology: conceptual synthesis reading NATO and scholarship; policy-inflected; moderate validity</t>
+  </si>
+  <si>
+    <t>D_Evaluate: strongest bite is 'zone not line' plus complementarity (p.11); Falsifier: if cross-case metrics show bright-line threshold or no blending</t>
+  </si>
+  <si>
+    <t>D_Author: editorial stance; OUP volume; policy-legal lens; audience is practitioners and scholars; Really saying: stabilise terms to enable strategy</t>
+  </si>
+  <si>
+    <t>D_Synthesis: aligns with NATO ambiguity and Mattis-Hoffman blending; diverges from 'buzzword' critiques by offering a usable definition</t>
+  </si>
+  <si>
+    <t>D_Limit: lacks thresholds and metrics; West-centric scope</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF should plan integrated statecraft and resilience below Article 5 triggers; set indicators for escalation control</t>
+  </si>
+  <si>
+    <t>Clementine G. Starling; Arun Iyer; Robert J. Giesler</t>
+  </si>
+  <si>
+    <t>Definition and practice of the 'gray zone'; autocracy advantage; democratic responses; US and allies</t>
+  </si>
+  <si>
+    <t>Expert Q&amp;A synthesis; policy commentary; practitioner perspectives (pp.1–4)</t>
+  </si>
+  <si>
+    <t>Gray-zone tactics proliferate; autocracies exploit asymmetry; democracies lag without whole-of-government strategy (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Definition spans non-military coercion, information ops, cyber, proxies; early action decisive; free press and alliances are assets (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Concise primer; multi-expert triangulation; concrete policy steps; links info, cyber, economic domains (pp.3–4)</t>
+  </si>
+  <si>
+    <t>Loose definition; scant evidence; US-centric lens; conflates hybrid war with broader influence (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Aligns with hybrid warfare literature on sub-threshold coercion; echoes deterrence by detection (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Downplays measurement and legal thresholds; privileges policy over empirics; treats autocracy advantage as given (pp.2–3)</t>
+  </si>
+  <si>
+    <t>Examples: Crimea, BRI leverage, Chinese islands, IRA disinfo; further reading links (pp.1,3–7)</t>
+  </si>
+  <si>
+    <t>Use as conceptual map only; build national playbook for detection, attribution, response; focus Irish DF on information and early action (pp.3–4)</t>
+  </si>
+  <si>
+    <t>Atlantic Council Forward Defense; pro-democracy, US policy audience; competition framing; normative emphasis on values (pp.1–4)</t>
+  </si>
+  <si>
+    <t>Pre-invasion timing; no metrics; ambiguous term; no EU small-state lens; not peer reviewed (pp.1–4)</t>
+  </si>
+  <si>
+    <t>Defines gray zone and argues democracies lag without strategy; early action matters (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Matters for small-state resilience; omits cost, legal risk, measurement of effectiveness</t>
+  </si>
+  <si>
+    <t>Q&amp;A expert synthesis with practitioner views; conceptual validity moderate; empirical base thin</t>
+  </si>
+  <si>
+    <t>Strongest bite: early response beats escalation (p.4); Falsifier: if delayed responses outperform early ones</t>
+  </si>
+  <si>
+    <t>Atlantic Council policy lens; Western values case; incentive to spur US action; Really saying: mobilise whole-of-government</t>
+  </si>
+  <si>
+    <t>Converges with hybrid warfare scholarship on sub-threshold coercion; diverges on definitional precision</t>
+  </si>
+  <si>
+    <t>No operational metrics; ambiguous scope; assumes autocracy advantage without counter-cases</t>
+  </si>
+  <si>
+    <t>Irish DF: invest in detection, attribution, allied messaging; codify rapid interagency playbooks; rehearse early moves</t>
+  </si>
+  <si>
+    <t>STARLING_2022</t>
+  </si>
+  <si>
+    <t>Chris Tuck</t>
+  </si>
+  <si>
+    <t>Hybrid War: The Perfect Enemy — critique of the hybrid warfare concept</t>
+  </si>
+  <si>
+    <t>Conceptual essay; critical synthesis of cases and commentary</t>
+  </si>
+  <si>
+    <t>Hybrid war label is over-broad, not distinct; reflects Western anxieties (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Definitional vagueness; generalising from specific; presentism; situational enablers; overestimating adversaries (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Clear critique; contrasts Crimea and Donbas; historical continuity; policy relevance (pp.2–4)</t>
+  </si>
+  <si>
+    <t>Blog-level rigour; sparse evidence; no operational definition; no metrics (pp.2–3)</t>
+  </si>
+  <si>
+    <t>Converges with Gray, Galeotti, van Puyvelde on continuity and caution (p.3)</t>
+  </si>
+  <si>
+    <t>Diverges from alarmist NATO discourse; challenges Hoffman and McCuen templates (p.2)</t>
+  </si>
+  <si>
+    <t>Crimea success relied on local factors; Donbas costly; “perfect enemy” line (pp.2,4)</t>
+  </si>
+  <si>
+    <t>Treat hybrid as lens not category; emphasise resilience and strategy; assess case by case (pp.2–4)</t>
+  </si>
+  <si>
+    <t>KCL Defence Studies context; incentive to puncture hype; policy-facing audience</t>
+  </si>
+  <si>
+    <t>No cross-case testing; limited sources; lacks falsifiable framework</t>
+  </si>
+  <si>
+    <t>Ill-defined hybrid war, context-bound, not a distinct form of war (pp.2–3)</t>
+  </si>
+  <si>
+    <t>Checks threat inflation; omits cases where hybrid produced durable strategic change</t>
+  </si>
+  <si>
+    <t>Blog essay; secondary synthesis; anecdotal examples; moderate validity</t>
+  </si>
+  <si>
+    <t>Strongest bite: presentism and Crimea–Donbas contrast (p.2); Falsifier: operational definition predicts cross-case success</t>
+  </si>
+  <si>
+    <t>Critical stance; KCL lens; policy audience. Really saying: fix strategy, not buzzwords</t>
+  </si>
+  <si>
+    <t>Aligns with Gray and van Puyvelde; diverges from Hoffman’s prescriptive model</t>
+  </si>
+  <si>
+    <t>No metrics or design tests; UK-centric lens</t>
+  </si>
+  <si>
+    <t>Irish DF prioritise deterrence by denial, cohesion, legal tools, tailored countermeasures</t>
+  </si>
+  <si>
+    <t>TUCK_2017</t>
   </si>
 </sst>
 </file>
@@ -13912,10 +14764,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111F966-AC4E-4B87-8117-CC0F46545464}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y174"/>
+  <dimension ref="A1:Y187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -26596,6 +27448,890 @@
         <v>4229</v>
       </c>
     </row>
+    <row r="175" spans="1:24">
+      <c r="A175" t="s">
+        <v>4252</v>
+      </c>
+      <c r="B175" t="s">
+        <v>4231</v>
+      </c>
+      <c r="C175" t="s">
+        <v>4232</v>
+      </c>
+      <c r="D175" t="s">
+        <v>4233</v>
+      </c>
+      <c r="E175" t="s">
+        <v>4234</v>
+      </c>
+      <c r="F175" t="s">
+        <v>4235</v>
+      </c>
+      <c r="G175" t="s">
+        <v>4236</v>
+      </c>
+      <c r="H175" t="s">
+        <v>4237</v>
+      </c>
+      <c r="I175" t="s">
+        <v>4238</v>
+      </c>
+      <c r="J175" t="s">
+        <v>4239</v>
+      </c>
+      <c r="K175" t="s">
+        <v>4240</v>
+      </c>
+      <c r="L175" t="s">
+        <v>4241</v>
+      </c>
+      <c r="M175" t="s">
+        <v>4242</v>
+      </c>
+      <c r="N175" t="s">
+        <v>4243</v>
+      </c>
+      <c r="O175" t="s">
+        <v>4244</v>
+      </c>
+      <c r="P175" t="s">
+        <v>4245</v>
+      </c>
+      <c r="Q175" t="s">
+        <v>4246</v>
+      </c>
+      <c r="R175" t="s">
+        <v>4247</v>
+      </c>
+      <c r="S175" t="s">
+        <v>4248</v>
+      </c>
+      <c r="T175" t="s">
+        <v>4249</v>
+      </c>
+      <c r="U175" t="s">
+        <v>4250</v>
+      </c>
+      <c r="V175" t="s">
+        <v>4251</v>
+      </c>
+    </row>
+    <row r="176" spans="1:24">
+      <c r="A176" t="s">
+        <v>4296</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4253</v>
+      </c>
+      <c r="C176" t="s">
+        <v>4254</v>
+      </c>
+      <c r="D176" t="s">
+        <v>4255</v>
+      </c>
+      <c r="E176" t="s">
+        <v>4256</v>
+      </c>
+      <c r="F176" t="s">
+        <v>4257</v>
+      </c>
+      <c r="G176" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H176" t="s">
+        <v>4259</v>
+      </c>
+      <c r="I176" t="s">
+        <v>4260</v>
+      </c>
+      <c r="J176" t="s">
+        <v>4261</v>
+      </c>
+      <c r="K176" t="s">
+        <v>4262</v>
+      </c>
+      <c r="L176" t="s">
+        <v>4263</v>
+      </c>
+      <c r="M176" t="s">
+        <v>4264</v>
+      </c>
+      <c r="N176" t="s">
+        <v>4265</v>
+      </c>
+      <c r="O176" t="s">
+        <v>4266</v>
+      </c>
+      <c r="P176" t="s">
+        <v>4267</v>
+      </c>
+      <c r="Q176" t="s">
+        <v>4268</v>
+      </c>
+      <c r="R176" t="s">
+        <v>4269</v>
+      </c>
+      <c r="S176" t="s">
+        <v>4270</v>
+      </c>
+      <c r="T176" t="s">
+        <v>4271</v>
+      </c>
+      <c r="U176" t="s">
+        <v>4272</v>
+      </c>
+      <c r="V176" t="s">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="177" spans="1:22">
+      <c r="A177" t="s">
+        <v>4295</v>
+      </c>
+      <c r="B177" t="s">
+        <v>4274</v>
+      </c>
+      <c r="C177" t="s">
+        <v>4275</v>
+      </c>
+      <c r="D177" t="s">
+        <v>4276</v>
+      </c>
+      <c r="E177" t="s">
+        <v>4277</v>
+      </c>
+      <c r="F177" t="s">
+        <v>4278</v>
+      </c>
+      <c r="G177" t="s">
+        <v>4279</v>
+      </c>
+      <c r="H177" t="s">
+        <v>4280</v>
+      </c>
+      <c r="I177" t="s">
+        <v>4281</v>
+      </c>
+      <c r="J177" t="s">
+        <v>4282</v>
+      </c>
+      <c r="K177" t="s">
+        <v>4283</v>
+      </c>
+      <c r="L177" t="s">
+        <v>4284</v>
+      </c>
+      <c r="M177" t="s">
+        <v>4285</v>
+      </c>
+      <c r="N177" t="s">
+        <v>4286</v>
+      </c>
+      <c r="O177" t="s">
+        <v>4287</v>
+      </c>
+      <c r="P177" t="s">
+        <v>4288</v>
+      </c>
+      <c r="Q177" t="s">
+        <v>4289</v>
+      </c>
+      <c r="R177" t="s">
+        <v>4290</v>
+      </c>
+      <c r="S177" t="s">
+        <v>4291</v>
+      </c>
+      <c r="T177" t="s">
+        <v>4292</v>
+      </c>
+      <c r="U177" t="s">
+        <v>4293</v>
+      </c>
+      <c r="V177" t="s">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="178" spans="1:22">
+      <c r="A178" t="s">
+        <v>4317</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4274</v>
+      </c>
+      <c r="C178" t="s">
+        <v>4297</v>
+      </c>
+      <c r="D178" t="s">
+        <v>4298</v>
+      </c>
+      <c r="E178" t="s">
+        <v>4299</v>
+      </c>
+      <c r="F178" t="s">
+        <v>4300</v>
+      </c>
+      <c r="G178" t="s">
+        <v>4301</v>
+      </c>
+      <c r="H178" t="s">
+        <v>4302</v>
+      </c>
+      <c r="I178" t="s">
+        <v>4303</v>
+      </c>
+      <c r="J178" t="s">
+        <v>4304</v>
+      </c>
+      <c r="K178" t="s">
+        <v>4305</v>
+      </c>
+      <c r="L178" t="s">
+        <v>4306</v>
+      </c>
+      <c r="M178" t="s">
+        <v>4307</v>
+      </c>
+      <c r="N178" t="s">
+        <v>4308</v>
+      </c>
+      <c r="O178" t="s">
+        <v>4309</v>
+      </c>
+      <c r="P178" t="s">
+        <v>4310</v>
+      </c>
+      <c r="Q178" t="s">
+        <v>4311</v>
+      </c>
+      <c r="R178" t="s">
+        <v>4312</v>
+      </c>
+      <c r="S178" t="s">
+        <v>4313</v>
+      </c>
+      <c r="T178" t="s">
+        <v>4314</v>
+      </c>
+      <c r="U178" t="s">
+        <v>4315</v>
+      </c>
+      <c r="V178" t="s">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="179" spans="1:22">
+      <c r="A179" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B179" t="s">
+        <v>4274</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4318</v>
+      </c>
+      <c r="D179" t="s">
+        <v>4319</v>
+      </c>
+      <c r="E179" t="s">
+        <v>4320</v>
+      </c>
+      <c r="F179" t="s">
+        <v>4321</v>
+      </c>
+      <c r="G179" t="s">
+        <v>4322</v>
+      </c>
+      <c r="H179" t="s">
+        <v>4323</v>
+      </c>
+      <c r="I179" t="s">
+        <v>4324</v>
+      </c>
+      <c r="J179" t="s">
+        <v>4325</v>
+      </c>
+      <c r="K179" t="s">
+        <v>4326</v>
+      </c>
+      <c r="L179" t="s">
+        <v>4327</v>
+      </c>
+      <c r="M179" t="s">
+        <v>4328</v>
+      </c>
+      <c r="N179" t="s">
+        <v>4329</v>
+      </c>
+      <c r="O179" t="s">
+        <v>4330</v>
+      </c>
+      <c r="P179" t="s">
+        <v>4331</v>
+      </c>
+      <c r="Q179" t="s">
+        <v>4332</v>
+      </c>
+      <c r="R179" t="s">
+        <v>4333</v>
+      </c>
+      <c r="S179" t="s">
+        <v>4334</v>
+      </c>
+      <c r="T179" t="s">
+        <v>4335</v>
+      </c>
+      <c r="U179" t="s">
+        <v>4336</v>
+      </c>
+      <c r="V179" t="s">
+        <v>4337</v>
+      </c>
+    </row>
+    <row r="180" spans="1:22">
+      <c r="A180" t="s">
+        <v>4360</v>
+      </c>
+      <c r="B180" t="s">
+        <v>4339</v>
+      </c>
+      <c r="C180" t="s">
+        <v>4340</v>
+      </c>
+      <c r="D180" t="s">
+        <v>4341</v>
+      </c>
+      <c r="E180" t="s">
+        <v>4342</v>
+      </c>
+      <c r="F180" t="s">
+        <v>4343</v>
+      </c>
+      <c r="G180" t="s">
+        <v>4344</v>
+      </c>
+      <c r="H180" t="s">
+        <v>4345</v>
+      </c>
+      <c r="I180" t="s">
+        <v>4346</v>
+      </c>
+      <c r="J180" t="s">
+        <v>4347</v>
+      </c>
+      <c r="K180" t="s">
+        <v>4348</v>
+      </c>
+      <c r="L180" t="s">
+        <v>4349</v>
+      </c>
+      <c r="M180" t="s">
+        <v>4350</v>
+      </c>
+      <c r="N180" t="s">
+        <v>4351</v>
+      </c>
+      <c r="O180" t="s">
+        <v>4352</v>
+      </c>
+      <c r="P180" t="s">
+        <v>4353</v>
+      </c>
+      <c r="Q180" t="s">
+        <v>4354</v>
+      </c>
+      <c r="R180" t="s">
+        <v>4355</v>
+      </c>
+      <c r="S180" t="s">
+        <v>4356</v>
+      </c>
+      <c r="T180" t="s">
+        <v>4357</v>
+      </c>
+      <c r="U180" t="s">
+        <v>4358</v>
+      </c>
+      <c r="V180" t="s">
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="181" spans="1:22">
+      <c r="A181" t="s">
+        <v>4514</v>
+      </c>
+      <c r="B181" t="s">
+        <v>4493</v>
+      </c>
+      <c r="C181" t="s">
+        <v>4494</v>
+      </c>
+      <c r="D181" t="s">
+        <v>4495</v>
+      </c>
+      <c r="E181" t="s">
+        <v>4496</v>
+      </c>
+      <c r="F181" t="s">
+        <v>4497</v>
+      </c>
+      <c r="G181" t="s">
+        <v>4498</v>
+      </c>
+      <c r="H181" t="s">
+        <v>4499</v>
+      </c>
+      <c r="I181" t="s">
+        <v>4500</v>
+      </c>
+      <c r="J181" t="s">
+        <v>4501</v>
+      </c>
+      <c r="K181" t="s">
+        <v>4502</v>
+      </c>
+      <c r="L181" t="s">
+        <v>4503</v>
+      </c>
+      <c r="M181" t="s">
+        <v>4504</v>
+      </c>
+      <c r="N181" t="s">
+        <v>4505</v>
+      </c>
+      <c r="O181" t="s">
+        <v>4506</v>
+      </c>
+      <c r="P181" t="s">
+        <v>4507</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>4508</v>
+      </c>
+      <c r="R181" t="s">
+        <v>4509</v>
+      </c>
+      <c r="S181" t="s">
+        <v>4510</v>
+      </c>
+      <c r="T181" t="s">
+        <v>4511</v>
+      </c>
+      <c r="U181" t="s">
+        <v>4512</v>
+      </c>
+      <c r="V181" t="s">
+        <v>4513</v>
+      </c>
+    </row>
+    <row r="182" spans="1:22">
+      <c r="A182" t="s">
+        <v>4448</v>
+      </c>
+      <c r="B182" t="s">
+        <v>4427</v>
+      </c>
+      <c r="C182" t="s">
+        <v>4428</v>
+      </c>
+      <c r="D182" t="s">
+        <v>4429</v>
+      </c>
+      <c r="E182" t="s">
+        <v>4430</v>
+      </c>
+      <c r="F182" t="s">
+        <v>4431</v>
+      </c>
+      <c r="G182" t="s">
+        <v>4432</v>
+      </c>
+      <c r="H182" t="s">
+        <v>4433</v>
+      </c>
+      <c r="I182" t="s">
+        <v>4434</v>
+      </c>
+      <c r="J182" t="s">
+        <v>4435</v>
+      </c>
+      <c r="K182" t="s">
+        <v>4436</v>
+      </c>
+      <c r="L182" t="s">
+        <v>4437</v>
+      </c>
+      <c r="M182" t="s">
+        <v>4438</v>
+      </c>
+      <c r="N182" t="s">
+        <v>4439</v>
+      </c>
+      <c r="O182" t="s">
+        <v>4440</v>
+      </c>
+      <c r="P182" t="s">
+        <v>4441</v>
+      </c>
+      <c r="Q182" t="s">
+        <v>4442</v>
+      </c>
+      <c r="R182" t="s">
+        <v>4443</v>
+      </c>
+      <c r="S182" t="s">
+        <v>4444</v>
+      </c>
+      <c r="T182" t="s">
+        <v>4445</v>
+      </c>
+      <c r="U182" t="s">
+        <v>4446</v>
+      </c>
+      <c r="V182" t="s">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="183" spans="1:22">
+      <c r="A183" t="s">
+        <v>4382</v>
+      </c>
+      <c r="B183" t="s">
+        <v>4361</v>
+      </c>
+      <c r="C183" t="s">
+        <v>4362</v>
+      </c>
+      <c r="D183" t="s">
+        <v>4363</v>
+      </c>
+      <c r="E183" t="s">
+        <v>4364</v>
+      </c>
+      <c r="F183" t="s">
+        <v>4365</v>
+      </c>
+      <c r="G183" t="s">
+        <v>4366</v>
+      </c>
+      <c r="H183" t="s">
+        <v>4367</v>
+      </c>
+      <c r="I183" t="s">
+        <v>4368</v>
+      </c>
+      <c r="J183" t="s">
+        <v>4369</v>
+      </c>
+      <c r="K183" t="s">
+        <v>4370</v>
+      </c>
+      <c r="L183" t="s">
+        <v>4371</v>
+      </c>
+      <c r="M183" t="s">
+        <v>4372</v>
+      </c>
+      <c r="N183" t="s">
+        <v>4373</v>
+      </c>
+      <c r="O183" t="s">
+        <v>4374</v>
+      </c>
+      <c r="P183" t="s">
+        <v>4375</v>
+      </c>
+      <c r="Q183" t="s">
+        <v>4376</v>
+      </c>
+      <c r="R183" t="s">
+        <v>4377</v>
+      </c>
+      <c r="S183" t="s">
+        <v>4378</v>
+      </c>
+      <c r="T183" t="s">
+        <v>4379</v>
+      </c>
+      <c r="U183" t="s">
+        <v>4380</v>
+      </c>
+      <c r="V183" t="s">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="184" spans="1:22">
+      <c r="A184" t="s">
+        <v>4404</v>
+      </c>
+      <c r="B184" t="s">
+        <v>4383</v>
+      </c>
+      <c r="C184" t="s">
+        <v>4384</v>
+      </c>
+      <c r="D184" t="s">
+        <v>4385</v>
+      </c>
+      <c r="E184" t="s">
+        <v>4386</v>
+      </c>
+      <c r="F184" t="s">
+        <v>4387</v>
+      </c>
+      <c r="G184" t="s">
+        <v>4388</v>
+      </c>
+      <c r="H184" t="s">
+        <v>4389</v>
+      </c>
+      <c r="I184" t="s">
+        <v>4390</v>
+      </c>
+      <c r="J184" t="s">
+        <v>4391</v>
+      </c>
+      <c r="K184" t="s">
+        <v>4392</v>
+      </c>
+      <c r="L184" t="s">
+        <v>4393</v>
+      </c>
+      <c r="M184" t="s">
+        <v>4394</v>
+      </c>
+      <c r="N184" t="s">
+        <v>4395</v>
+      </c>
+      <c r="O184" t="s">
+        <v>4396</v>
+      </c>
+      <c r="P184" t="s">
+        <v>4397</v>
+      </c>
+      <c r="Q184" t="s">
+        <v>4398</v>
+      </c>
+      <c r="R184" t="s">
+        <v>4399</v>
+      </c>
+      <c r="S184" t="s">
+        <v>4400</v>
+      </c>
+      <c r="T184" t="s">
+        <v>4401</v>
+      </c>
+      <c r="U184" t="s">
+        <v>4402</v>
+      </c>
+      <c r="V184" t="s">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="185" spans="1:22">
+      <c r="A185" t="s">
+        <v>4426</v>
+      </c>
+      <c r="B185" t="s">
+        <v>4405</v>
+      </c>
+      <c r="C185" t="s">
+        <v>4406</v>
+      </c>
+      <c r="D185" t="s">
+        <v>4407</v>
+      </c>
+      <c r="E185" t="s">
+        <v>4408</v>
+      </c>
+      <c r="F185" t="s">
+        <v>4409</v>
+      </c>
+      <c r="G185" t="s">
+        <v>4410</v>
+      </c>
+      <c r="H185" t="s">
+        <v>4411</v>
+      </c>
+      <c r="I185" t="s">
+        <v>4412</v>
+      </c>
+      <c r="J185" t="s">
+        <v>4413</v>
+      </c>
+      <c r="K185" t="s">
+        <v>4414</v>
+      </c>
+      <c r="L185" t="s">
+        <v>4415</v>
+      </c>
+      <c r="M185" t="s">
+        <v>4416</v>
+      </c>
+      <c r="N185" t="s">
+        <v>4417</v>
+      </c>
+      <c r="O185" t="s">
+        <v>4418</v>
+      </c>
+      <c r="P185" t="s">
+        <v>4419</v>
+      </c>
+      <c r="Q185" t="s">
+        <v>4420</v>
+      </c>
+      <c r="R185" t="s">
+        <v>4421</v>
+      </c>
+      <c r="S185" t="s">
+        <v>4422</v>
+      </c>
+      <c r="T185" t="s">
+        <v>4423</v>
+      </c>
+      <c r="U185" t="s">
+        <v>4424</v>
+      </c>
+      <c r="V185" t="s">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="186" spans="1:22">
+      <c r="A186" t="s">
+        <v>4449</v>
+      </c>
+      <c r="B186" t="s">
+        <v>4450</v>
+      </c>
+      <c r="C186" t="s">
+        <v>4451</v>
+      </c>
+      <c r="D186" t="s">
+        <v>4452</v>
+      </c>
+      <c r="E186" t="s">
+        <v>4453</v>
+      </c>
+      <c r="F186" t="s">
+        <v>4454</v>
+      </c>
+      <c r="G186" t="s">
+        <v>4455</v>
+      </c>
+      <c r="H186" t="s">
+        <v>4456</v>
+      </c>
+      <c r="I186" t="s">
+        <v>4457</v>
+      </c>
+      <c r="J186" t="s">
+        <v>4458</v>
+      </c>
+      <c r="K186" t="s">
+        <v>4459</v>
+      </c>
+      <c r="L186" t="s">
+        <v>4460</v>
+      </c>
+      <c r="M186" t="s">
+        <v>4461</v>
+      </c>
+      <c r="N186" t="s">
+        <v>4462</v>
+      </c>
+      <c r="O186" t="s">
+        <v>4463</v>
+      </c>
+      <c r="P186" t="s">
+        <v>4464</v>
+      </c>
+      <c r="Q186" t="s">
+        <v>4465</v>
+      </c>
+      <c r="R186" t="s">
+        <v>4466</v>
+      </c>
+      <c r="S186" t="s">
+        <v>4467</v>
+      </c>
+      <c r="T186" t="s">
+        <v>4468</v>
+      </c>
+      <c r="U186" t="s">
+        <v>4469</v>
+      </c>
+      <c r="V186" t="s">
+        <v>4470</v>
+      </c>
+    </row>
+    <row r="187" spans="1:22">
+      <c r="A187" t="s">
+        <v>4492</v>
+      </c>
+      <c r="B187" t="s">
+        <v>4471</v>
+      </c>
+      <c r="C187" t="s">
+        <v>4472</v>
+      </c>
+      <c r="D187" t="s">
+        <v>4473</v>
+      </c>
+      <c r="E187" t="s">
+        <v>4474</v>
+      </c>
+      <c r="F187" t="s">
+        <v>4475</v>
+      </c>
+      <c r="G187" t="s">
+        <v>4476</v>
+      </c>
+      <c r="H187" t="s">
+        <v>4477</v>
+      </c>
+      <c r="I187" t="s">
+        <v>4478</v>
+      </c>
+      <c r="J187" t="s">
+        <v>4479</v>
+      </c>
+      <c r="K187" t="s">
+        <v>4480</v>
+      </c>
+      <c r="L187" t="s">
+        <v>4481</v>
+      </c>
+      <c r="M187" t="s">
+        <v>4482</v>
+      </c>
+      <c r="N187" t="s">
+        <v>4483</v>
+      </c>
+      <c r="O187" t="s">
+        <v>4484</v>
+      </c>
+      <c r="P187" t="s">
+        <v>4485</v>
+      </c>
+      <c r="Q187" t="s">
+        <v>4486</v>
+      </c>
+      <c r="R187" t="s">
+        <v>4487</v>
+      </c>
+      <c r="S187" t="s">
+        <v>4488</v>
+      </c>
+      <c r="T187" t="s">
+        <v>4489</v>
+      </c>
+      <c r="U187" t="s">
+        <v>4490</v>
+      </c>
+      <c r="V187" t="s">
+        <v>4491</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y171">
     <sortCondition ref="A2:A171"/>

</xml_diff>

<commit_message>
presentation and DSS work
</commit_message>
<xml_diff>
--- a/JCSC_SOURCE_MATRIX.xlsx
+++ b/JCSC_SOURCE_MATRIX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\JCSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF29973-8350-4060-A16A-81FB15761772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2FCA59-B371-493A-9802-700C05D82F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{9A08C367-70A1-4CB7-9B0B-0DF2B9CEDD0C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="4777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4901" uniqueCount="4821">
   <si>
     <t>Author</t>
   </si>
@@ -15121,6 +15121,138 @@
   </si>
   <si>
     <t>SNIDER_2000</t>
+  </si>
+  <si>
+    <t>Patricia M. Shields</t>
+  </si>
+  <si>
+    <t>Afghanistan’s imprint on AF&amp;S content; postmodern military lens</t>
+  </si>
+  <si>
+    <t>Editor’s reflection; narrative content analysis over 2001–2021</t>
+  </si>
+  <si>
+    <t>Afghanistan shifted AF&amp;S toward reserves, contractors, ISAF management, health and family stress; civil–military effects were indirect (pp. 893–902)</t>
+  </si>
+  <si>
+    <t>Postmodern force, multinational ISAF, rise in veterans’ health, reserve reliance, contracting, small wars, public opinion; stewardship metaphor (pp. 893–901)</t>
+  </si>
+  <si>
+    <t>Editor vantage over full war; coherent mapping of themes; international breadth; links to Moskos–Williams–Segal (pp. 893–896; 900–901)</t>
+  </si>
+  <si>
+    <t>Not a formal scoping review; limited metrics; conflates Iraq with Afghanistan at points; selection effects (pp. 893–894; 902)</t>
+  </si>
+  <si>
+    <t>Converges with postmodern military theses and family/health literatures</t>
+  </si>
+  <si>
+    <t>Diverts from tech-centric RMA narratives by privileging social-institutional shifts</t>
+  </si>
+  <si>
+    <t>Use Afghan-era patterns to weight DSS topics: mental health, reserves, contractors, intercultural competence, public legitimacy (pp. 896–901)</t>
+  </si>
+  <si>
+    <t>Irish DF PME and research should treat LOAC-health-family-reserves as core, and plan for coalition complexity (pp. 896–901)</t>
+  </si>
+  <si>
+    <t>Editor–in–chief lens; stewardship incentives; US-led coalition context; Really saying: the war re-grew the field’s forest</t>
+  </si>
+  <si>
+    <t>Commentary, not causal identification; no bibliometrics or counterfactual tests (pp. 893–894)</t>
+  </si>
+  <si>
+    <t>D_Describe: Twenty-year Afghan war reoriented AF&amp;S toward reserves, contractors, ISAF, health, families; CMR shifts were indirect (pp. 893–901).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Matters to DSS because it reprioritises what militaries actually grappled with; omits quantified effect sizes.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Editorial narrative over the journal’s corpus; validity thematic, not statistical; Iraq folded in.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest bite is the concrete catalogue of shifts and their timing; Falsifier: if bibliometrics show no post-2015 health/family surge.</t>
+  </si>
+  <si>
+    <t>D_Author: Long-tenure editor, pragmatic–postmodern lens; Really saying: Afghanistan changed the journal’s climate.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with Moskos et al. on postmodern militaries and with Forster on politicisation.</t>
+  </si>
+  <si>
+    <t>D_Limit: Commentary genre and US–NATO tilt.</t>
+  </si>
+  <si>
+    <t>D_Implication: DF should weight PME toward health, families, reserves, contractors, and coalition skills, not just kinetic.</t>
+  </si>
+  <si>
+    <t>SHIELDS_2002</t>
+  </si>
+  <si>
+    <t>Bradford Booth; Meyer Kestnbaum; David R. Segal</t>
+  </si>
+  <si>
+    <t>Are Post-Cold War Militaries Postmodern?</t>
+  </si>
+  <si>
+    <t>Conceptual critique and theoretical synthesis; engages postindustrialism, post-Fordism, globalisation; Baudrillard illustration</t>
+  </si>
+  <si>
+    <t>Civil–military change reflects postmodern conditions but militaries respond with modern, rational adaptation; “postmodern military” overstates novelty (pp.320–333; 337–338)</t>
+  </si>
+  <si>
+    <t>Postindustrialism–post-Fordism–globalisation map to Moskos’ dimensions; mission shift has no postmodern strand; geopolitics central; bureaucracy and citizenship persist; simulation and hyperreality shape perception (pp.324–329; 330–336)</t>
+  </si>
+  <si>
+    <t>Clear terms; bridges theory to observed traits; highlights continuity with Weberian bureaucracy; offers alternative criteria via media, simulacra; policy-relevant caution (pp.324–336)</t>
+  </si>
+  <si>
+    <t>No systematic tests; US-centric touchstones; secondary sources; thin operationalisation; “postmodern” contested (pp.321–323; 330–333)</t>
+  </si>
+  <si>
+    <t>Converges with Dandeker on adaptive restructuring; aligns with Burk on transnational frames; complements Betts on spectacle and escalation optics</t>
+  </si>
+  <si>
+    <t>Differs from Moskos’ postmodern typology; stresses geopolitics and gradualism over rupture (pp.321–323; 328–330)</t>
+  </si>
+  <si>
+    <t>Distinguishes postmodernity (epoch) from postmodernism (discourse); outlines decline of mass army; marginalisation trend; media feedback loops in operations (pp.324–338)</t>
+  </si>
+  <si>
+    <t>Use late-modern lens for Irish DF; adapt to postmodern conditions; add media-simulation governance and coalition design checks (pp.330–338)</t>
+  </si>
+  <si>
+    <t>Academic sociological lens; ARI-supported work; incentive to discipline fashionable labels and recentre evidence</t>
+  </si>
+  <si>
+    <t>Conceptual essay; scarce cross-national data; no measurement recipe; examples impressionistic</t>
+  </si>
+  <si>
+    <t>D_Describe: Postmodern conditions spur modern organisational adaptation; the “postmodern military” label is premature (pp.320–333).</t>
+  </si>
+  <si>
+    <t>D_Interpret: Labels drive policy and metrics; mislabelling risks shallow reforms; measurement guidance is absent.</t>
+  </si>
+  <si>
+    <t>D_Methodology: Theory mapping to three macro-processes; critique of mission shift; Baudrillard as lens; moderate validity.</t>
+  </si>
+  <si>
+    <t>D_Evaluate: Strongest bite is the modernity-through-adaptation claim with geopolitics as driver (pp.328–333); Falsifier: cross-cases where postmodern mechanisms, not geopolitics, predict structure.</t>
+  </si>
+  <si>
+    <t>D_Author: University of Maryland CRMO; contract support; Really saying: environment may be postmodern, militaries remain modern.</t>
+  </si>
+  <si>
+    <t>D_Synthesis: Aligns with Kuehn–Lorenz on specifying actors and linkage; tempers Moskos; complements Betts on spectacle risk.</t>
+  </si>
+  <si>
+    <t>D_Limit: Illustrative not systematic; concept borders blur.</t>
+  </si>
+  <si>
+    <t>D_Implication: Irish DF should keep late-modern design, add media–simulation controls and coalition layers; align with DSS LO on theory critique and testable claims.</t>
+  </si>
+  <si>
+    <t>BOOTH_2001</t>
   </si>
 </sst>
 </file>
@@ -15550,10 +15682,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111F966-AC4E-4B87-8117-CC0F46545464}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y199"/>
+  <dimension ref="A1:Y201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A182" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200"/>
+      <selection activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -29931,6 +30063,142 @@
         <v>4775</v>
       </c>
     </row>
+    <row r="200" spans="1:23">
+      <c r="A200" t="s">
+        <v>4798</v>
+      </c>
+      <c r="B200" t="s">
+        <v>4777</v>
+      </c>
+      <c r="C200" t="s">
+        <v>4778</v>
+      </c>
+      <c r="D200" t="s">
+        <v>4779</v>
+      </c>
+      <c r="E200" t="s">
+        <v>4780</v>
+      </c>
+      <c r="F200" t="s">
+        <v>4781</v>
+      </c>
+      <c r="G200" t="s">
+        <v>4782</v>
+      </c>
+      <c r="H200" t="s">
+        <v>4783</v>
+      </c>
+      <c r="I200" t="s">
+        <v>4784</v>
+      </c>
+      <c r="J200" t="s">
+        <v>4785</v>
+      </c>
+      <c r="K200" t="s">
+        <v>4786</v>
+      </c>
+      <c r="L200" t="s">
+        <v>4787</v>
+      </c>
+      <c r="M200" t="s">
+        <v>4788</v>
+      </c>
+      <c r="N200" t="s">
+        <v>4789</v>
+      </c>
+      <c r="O200" t="s">
+        <v>4790</v>
+      </c>
+      <c r="P200" t="s">
+        <v>4791</v>
+      </c>
+      <c r="Q200" t="s">
+        <v>4792</v>
+      </c>
+      <c r="R200" t="s">
+        <v>4793</v>
+      </c>
+      <c r="S200" t="s">
+        <v>4794</v>
+      </c>
+      <c r="T200" t="s">
+        <v>4795</v>
+      </c>
+      <c r="U200" t="s">
+        <v>4796</v>
+      </c>
+      <c r="V200" t="s">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="201" spans="1:23">
+      <c r="A201" t="s">
+        <v>4820</v>
+      </c>
+      <c r="B201" t="s">
+        <v>4799</v>
+      </c>
+      <c r="C201" t="s">
+        <v>4800</v>
+      </c>
+      <c r="D201" t="s">
+        <v>4801</v>
+      </c>
+      <c r="E201" t="s">
+        <v>4802</v>
+      </c>
+      <c r="F201" t="s">
+        <v>4803</v>
+      </c>
+      <c r="G201" t="s">
+        <v>4804</v>
+      </c>
+      <c r="H201" t="s">
+        <v>4805</v>
+      </c>
+      <c r="I201" t="s">
+        <v>4806</v>
+      </c>
+      <c r="J201" t="s">
+        <v>4807</v>
+      </c>
+      <c r="K201" t="s">
+        <v>4808</v>
+      </c>
+      <c r="L201" t="s">
+        <v>4809</v>
+      </c>
+      <c r="M201" t="s">
+        <v>4810</v>
+      </c>
+      <c r="N201" t="s">
+        <v>4811</v>
+      </c>
+      <c r="O201" t="s">
+        <v>4812</v>
+      </c>
+      <c r="P201" t="s">
+        <v>4813</v>
+      </c>
+      <c r="Q201" t="s">
+        <v>4814</v>
+      </c>
+      <c r="R201" t="s">
+        <v>4815</v>
+      </c>
+      <c r="S201" t="s">
+        <v>4816</v>
+      </c>
+      <c r="T201" t="s">
+        <v>4817</v>
+      </c>
+      <c r="U201" t="s">
+        <v>4818</v>
+      </c>
+      <c r="V201" t="s">
+        <v>4819</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y170">
     <sortCondition ref="A2:A170"/>

</xml_diff>